<commit_message>
Casos de modulo maestros listos
</commit_message>
<xml_diff>
--- a/Maestros.xlsx
+++ b/Maestros.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="540">
   <si>
     <t>Nombre CP</t>
   </si>
@@ -1251,9 +1251,6 @@
     <t>TC_Cartera_TipoGestion_Modificar</t>
   </si>
   <si>
-    <t>TC_Cartera_MotivoRecompra_ConsolidadoError</t>
-  </si>
-  <si>
     <t>TC_Cartera_UbicacionesVehiculos_AgregarConsulta</t>
   </si>
   <si>
@@ -1634,6 +1631,48 @@
   </si>
   <si>
     <t>Validar funcionalidad eliminar de registro exitente en formulario motivo recompra pestaña carta guia, seleccionando registro que puede ser eliminado.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para ingresar  al modulo Maestro, sub-modulo motivo recompra, hacer en enlace recompra descripcion, hacer clic en pestaña carta guia, hacer clic en icono eliminar.</t>
+  </si>
+  <si>
+    <t>Sistema emite mensaje indicando que no es posible eliminar registro.</t>
+  </si>
+  <si>
+    <t>Validar consulta del formulario motivo recompra pestaña carta guia, luego de acceder al mismo a través de enlace recompra descripción - enlace nomina pestaña pagares para finalizar con la descarga de archivo PDF.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para ingresar  al modulo Maestro, sub-modulo motivo recompra, hacer en enlace recompra descripcion, hacer clic en pestaña carta guia, hacer clic en enlace nomina, ingresar a pestaña pagares, hacer clic en boton generar PDF.</t>
+  </si>
+  <si>
+    <t>Descar de archivo de manera exitosa.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para ingresar  al modulo Maestro, sub-modulo motivo recompra, hacer en enlace recompra descripcion, hacer clic en pestaña carta guia, hacer clic en enlace ubicación pagare pestaña general, hacer clic en botón modificar.</t>
+  </si>
+  <si>
+    <t>Sistema permite la modificación de ubicación de pagare asociado a registro motivo recompra</t>
+  </si>
+  <si>
+    <t>Validar consulta de ubicación pagare, accediendo a traves de enlace ubicación pagare (fomulario motivo recompra, enlace recompra descripción pestaña carta guia), finalizando con la modificación y/o eliminación de registro.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para ingresar  al modulo Maestro, sub-modulo motivo recompra, hacer en enlace recompra descripcion, hacer clic en pestaña carta guia, hacer clic en enlace ubicación fisica pestaña general, hacer clic en botón eliminar.</t>
+  </si>
+  <si>
+    <t>Sistema permite la eliminación de ubicación de fisica asociado a registro motivo recompra</t>
+  </si>
+  <si>
+    <t>Validar consulta de ubicación fisica, accediendo a traves de enlace ubicación fisica (fomulario motivo recompra, enlace recompra descripción pestaña carta guia), finalizando con la eliminación de registro.</t>
+  </si>
+  <si>
+    <t>Validar consulta de motivo traslado, accediendo a traves de enlace motivo traslado (fomulario motivo recompra, enlace recompra descripción pestaña carta guia), finalizando con la modificación y eliminación de registro.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para ingresar  al modulo Maestro, sub-modulo motivo recompra, hacer en enlace recompra descripcion, hacer clic en pestaña carta guia, hacer clic en enlace motivo traslado pestaña general, hacer clic en botón modificar, luego de ello, proceder a eliminar registro haciendo clic en boton eliminar.</t>
+  </si>
+  <si>
+    <t>Sistema permite la modificación y eliminación de motivo traslados asociado a registro motivo recompra.</t>
   </si>
 </sst>
 </file>
@@ -10605,7 +10644,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B1" s="47" t="s">
         <v>5</v>
@@ -10685,10 +10724,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K3" s="12" t="str">
         <f>CONCATENATE("Validar funcionalidad ",IF(B3=1,$B$2,IF(C3=1,$C$2,IF(D3=1,$D$2)))," del modulo Maestro, sub-modulo Ubicaciones Vehiculos",IF(E3=1,", considerando la opcion exportar a excel",""),IF(F3=1,", hacer clic en enlace Descripción para modificar registro",IF(G3=1,", hacer clic en enlace Descripción para eliminar registro","")),IF(H3=1,", finalizando con la consulta mediante el filtro ",""),IF(H3=1,$H$2,""),IF(H3=1," con el dato ",""),IF(H3=1,I3,""))</f>
@@ -10722,10 +10761,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K4" s="12" t="str">
         <f t="shared" ref="K4:K17" si="0">CONCATENATE("Validar funcionalidad ",IF(B4=1,$B$2,IF(C4=1,$C$2,IF(D4=1,$D$2)))," del modulo Maestro, sub-modulo Ubicaciones Vehiculos",IF(E4=1,", considerando la opcion exportar a excel",""),IF(F4=1,", hacer clic en enlace Descripción para modificar registro",IF(G4=1,", hacer clic en enlace Descripción para eliminar registro","")),IF(H4=1,", finalizando con la consulta mediante el filtro ",""),IF(H4=1,$H$2,""),IF(H4=1," con el dato ",""),IF(H4=1,I4,""))</f>
@@ -10756,7 +10795,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="10"/>
       <c r="J5" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="K5" s="12" t="str">
         <f t="shared" si="0"/>
@@ -10789,7 +10828,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="10"/>
       <c r="J6" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K6" s="12" t="str">
         <f t="shared" si="0"/>
@@ -10818,7 +10857,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="10"/>
       <c r="J7" s="7" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K7" s="12" t="str">
         <f t="shared" si="0"/>
@@ -10854,7 +10893,7 @@
         <v>371</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K8" s="12" t="str">
         <f t="shared" si="0"/>
@@ -10887,10 +10926,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K9" s="12" t="str">
         <f t="shared" si="0"/>
@@ -10919,7 +10958,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
       <c r="J10" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K10" s="12" t="str">
         <f t="shared" si="0"/>
@@ -10951,7 +10990,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="10"/>
       <c r="J11" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K11" s="12" t="str">
         <f t="shared" si="0"/>
@@ -10978,7 +11017,7 @@
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
       <c r="J12" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K12" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11010,10 +11049,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K13" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11045,10 +11084,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K14" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11076,7 +11115,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="22"/>
       <c r="J15" s="7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K15" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11107,7 +11146,7 @@
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K16" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11133,7 +11172,7 @@
       <c r="H17" s="9"/>
       <c r="I17" s="10"/>
       <c r="J17" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K17" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11241,13 +11280,13 @@
       <c r="H24" s="9"/>
       <c r="I24" s="10"/>
       <c r="J24" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K24" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="L24" s="39" t="s">
         <v>417</v>
-      </c>
-      <c r="L24" s="39" t="s">
-        <v>418</v>
       </c>
       <c r="M24" s="7" t="s">
         <v>299</v>
@@ -11590,7 +11629,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B1" s="47" t="s">
         <v>5</v>
@@ -11635,19 +11674,19 @@
       </c>
       <c r="E2" s="44"/>
       <c r="F2" s="40" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>39</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>376</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K2" s="44"/>
       <c r="L2" s="44"/>
@@ -11678,7 +11717,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L3" s="12" t="str">
         <f>CONCATENATE("Validar funcionalidad ",IF(B3=1,$B$2,IF(C3=1,$C$2,IF(D3=1,$D$2)))," del modulo Maestro, sub-modulo Usuarios Empresas Externas",IF(E3=1,", considerando la opcion exportar a excel",""),IF(F3=1,", hacer clic en enlace Email para abrir ventada de envio de correo",""),IF(G3=1,", finalizando con la consulta mediante el filtro(s) ",""),IF(G3=1,$G$2,"")," ",IF(H3=1,$H$2,"")," ",IF(I3=1,$I$2,"")," ",IF(J3=1,$J$2,""))</f>
@@ -11710,7 +11749,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="L4" s="12" t="str">
         <f t="shared" ref="L4:L17" si="0">CONCATENATE("Validar funcionalidad ",IF(B4=1,$B$2,IF(C4=1,$C$2,IF(D4=1,$D$2)))," del modulo Maestro, sub-modulo Usuarios Empresas Externas",IF(E4=1,", considerando la opcion exportar a excel",""),IF(F4=1,", hacer clic en enlace Email para abrir ventada de envio de correo",""),IF(G4=1,", finalizando con la consulta mediante el filtro(s) ",""),IF(G4=1,$G$2,"")," ",IF(H4=1,$H$2,"")," ",IF(I4=1,$I$2,"")," ",IF(J4=1,$J$2,""))</f>
@@ -11746,7 +11785,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L5" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11778,7 +11817,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L6" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11812,7 +11851,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L7" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11845,7 +11884,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="L8" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11880,7 +11919,7 @@
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="L9" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11914,7 +11953,7 @@
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L10" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11949,7 +11988,7 @@
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L11" s="12" t="str">
         <f t="shared" si="0"/>
@@ -11981,7 +12020,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L12" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12013,7 +12052,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L13" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12043,7 +12082,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L14" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12072,7 +12111,7 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L15" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12102,7 +12141,7 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L16" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12129,7 +12168,7 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L17" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12244,13 +12283,13 @@
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L24" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="M24" s="39" t="s">
         <v>436</v>
-      </c>
-      <c r="M24" s="39" t="s">
-        <v>437</v>
       </c>
       <c r="N24" s="7" t="s">
         <v>299</v>
@@ -12619,7 +12658,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B1" s="47" t="s">
         <v>5</v>
@@ -12630,7 +12669,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G1" s="49"/>
       <c r="H1" s="52" t="s">
@@ -12669,10 +12708,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>446</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>447</v>
       </c>
       <c r="J2" s="44"/>
       <c r="K2" s="44"/>
@@ -12700,7 +12739,7 @@
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K3" s="12" t="str">
         <f>CONCATENATE("Validar funcionalidad ",IF(B3=1,$B$2,IF(C3=1,$C$2,IF(D3=1,$D$2)))," del modulo Maestro, sub-modulo Tipo Procesos",IF(E3=1,", considerando la opcion exportar a excel",""),IF(F3=1,", hacer clic en enlace Acronimo para modificar registro",IF(G3=1,", hacer clic en enlace Acronimo para eliminar registro","")),IF(H3=1,", finalizando con la consulta mediante el filtro ",""),IF(H3=1,$H$2,""),IF(I3=1,$I$2,""))</f>
@@ -12735,7 +12774,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K4" s="12" t="str">
         <f t="shared" ref="K4:K17" si="0">CONCATENATE("Validar funcionalidad ",IF(B4=1,$B$2,IF(C4=1,$C$2,IF(D4=1,$D$2)))," del modulo Maestro, sub-modulo Tipo Procesos",IF(E4=1,", considerando la opcion exportar a excel",""),IF(F4=1,", hacer clic en enlace Acronimo para modificar registro",IF(G4=1,", hacer clic en enlace Acronimo para eliminar registro","")),IF(H4=1,", finalizando con la consulta mediante el filtro ",""),IF(H4=1,$H$2,""),IF(I4=1,$I$2,""))</f>
@@ -12768,7 +12807,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K5" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12805,7 +12844,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K6" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12836,7 +12875,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K7" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12870,7 +12909,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K8" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12906,7 +12945,7 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K9" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12939,7 +12978,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K10" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12973,7 +13012,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K11" s="12" t="str">
         <f t="shared" si="0"/>
@@ -13002,7 +13041,7 @@
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K12" s="12" t="str">
         <f t="shared" si="0"/>
@@ -13035,7 +13074,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K13" s="12" t="str">
         <f t="shared" si="0"/>
@@ -13072,7 +13111,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K14" s="12" t="str">
         <f t="shared" si="0"/>
@@ -13102,7 +13141,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K15" s="12" t="str">
         <f t="shared" si="0"/>
@@ -13135,7 +13174,7 @@
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K16" s="12" t="str">
         <f t="shared" si="0"/>
@@ -13163,7 +13202,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K17" s="12" t="str">
         <f t="shared" si="0"/>
@@ -13273,13 +13312,13 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K24" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="L24" s="39" t="s">
         <v>465</v>
-      </c>
-      <c r="L24" s="39" t="s">
-        <v>466</v>
       </c>
       <c r="M24" s="7" t="s">
         <v>299</v>
@@ -14771,16 +14810,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14814,7 +14853,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B1" s="47" t="s">
         <v>5</v>
@@ -14825,7 +14864,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G1" s="49"/>
       <c r="H1" s="52" t="s">
@@ -14864,7 +14903,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I2" s="19" t="s">
         <v>14</v>
@@ -14894,10 +14933,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K3" s="12" t="str">
         <f>CONCATENATE("Validar funcionalidad ",IF(B3=1,$B$2,IF(C3=1,$C$2,IF(D3=1,$D$2)))," del modulo Maestro, sub-modulo CIA GPS",IF(E3=1,", considerando la opcion exportar a excel",""),IF(F3=1,", hacer clic en enlace CIA GPS para modificar registro",IF(G3=1,", hacer clic en enlace CIA GPS para eliminar registro","")),IF(H3=1,", finalizando con la consulta mediante el filtro ",""),IF(H3=1,$H$2,""),IF(H3=1," con el dato ",""),IF(H3=1,I3,""))</f>
@@ -14934,7 +14973,7 @@
         <v>371</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K4" s="12" t="str">
         <f t="shared" ref="K4:K17" si="0">CONCATENATE("Validar funcionalidad ",IF(B4=1,$B$2,IF(C4=1,$C$2,IF(D4=1,$D$2)))," del modulo Maestro, sub-modulo CIA GPS",IF(E4=1,", considerando la opcion exportar a excel",""),IF(F4=1,", hacer clic en enlace CIA GPS para modificar registro",IF(G4=1,", hacer clic en enlace CIA GPS para eliminar registro","")),IF(H4=1,", finalizando con la consulta mediante el filtro ",""),IF(H4=1,$H$2,""),IF(H4=1," con el dato ",""),IF(H4=1,I4,""))</f>
@@ -14965,7 +15004,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="10"/>
       <c r="J5" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K5" s="12" t="str">
         <f t="shared" si="0"/>
@@ -14998,7 +15037,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="10"/>
       <c r="J6" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K6" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15027,7 +15066,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="10"/>
       <c r="J7" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K7" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15060,10 +15099,10 @@
         <v>1</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K8" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15099,7 +15138,7 @@
         <v>5</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K9" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15128,7 +15167,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
       <c r="J10" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K10" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15160,7 +15199,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="10"/>
       <c r="J11" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K11" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15187,7 +15226,7 @@
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
       <c r="J12" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K12" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15219,10 +15258,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K13" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15257,7 +15296,7 @@
         <v>372</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K14" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15285,7 +15324,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="22"/>
       <c r="J15" s="7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K15" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15316,7 +15355,7 @@
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K16" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15342,7 +15381,7 @@
       <c r="H17" s="9"/>
       <c r="I17" s="10"/>
       <c r="J17" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K17" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15450,13 +15489,13 @@
       <c r="H24" s="9"/>
       <c r="I24" s="10"/>
       <c r="J24" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="K24" s="12" t="s">
         <v>486</v>
       </c>
-      <c r="K24" s="12" t="s">
+      <c r="L24" s="39" t="s">
         <v>487</v>
-      </c>
-      <c r="L24" s="39" t="s">
-        <v>488</v>
       </c>
       <c r="M24" s="7" t="s">
         <v>299</v>
@@ -15802,7 +15841,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B1" s="47" t="s">
         <v>5</v>
@@ -15856,10 +15895,10 @@
         <v>45</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K2" s="44"/>
       <c r="L2" s="44"/>
@@ -15888,7 +15927,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="23"/>
       <c r="K3" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L3" s="12" t="str">
         <f>CONCATENATE("Validar funcionalidad ",IF(B3=1,$B$2,IF(C3=1,$C$2,IF(D3=1,$D$2)))," del modulo Maestro, sub-modulo Documentos por Proveedor",IF(E3=1,", considerando la opcion exportar a excel",""),IF(F3=1,", hacer clic en enlace Descripción para modificar registro",IF(G3=1,", hacer clic en enlace Descripción para eliminar registro","")),IF(H3=1,", finalizando con la consulta mediante el filtro ",""),IF(H3=1,$H$2,""),IF(I3=1,$I$2,""),IF(J3=1,$J$2,""))</f>
@@ -15924,7 +15963,7 @@
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L4" s="12" t="str">
         <f t="shared" ref="L4:L17" si="0">CONCATENATE("Validar funcionalidad ",IF(B4=1,$B$2,IF(C4=1,$C$2,IF(D4=1,$D$2)))," del modulo Maestro, sub-modulo Documentos por Proveedor",IF(E4=1,", considerando la opcion exportar a excel",""),IF(F4=1,", hacer clic en enlace Descripción para modificar registro",IF(G4=1,", hacer clic en enlace Descripción para eliminar registro","")),IF(H4=1,", finalizando con la consulta mediante el filtro ",""),IF(H4=1,$H$2,""),IF(I4=1,$I$2,""),IF(J4=1,$J$2,""))</f>
@@ -15958,7 +15997,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L5" s="12" t="str">
         <f t="shared" si="0"/>
@@ -15992,7 +16031,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="10"/>
       <c r="K6" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L6" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16028,7 +16067,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L7" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16061,7 +16100,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="23"/>
       <c r="K8" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L8" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16096,7 +16135,7 @@
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L9" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16128,7 +16167,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L10" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16163,7 +16202,7 @@
       <c r="I11" s="9"/>
       <c r="J11" s="10"/>
       <c r="K11" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L11" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16191,7 +16230,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="10"/>
       <c r="K12" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="L12" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16225,7 +16264,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="L13" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16259,7 +16298,7 @@
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="L14" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16290,7 +16329,7 @@
       <c r="I15" s="9"/>
       <c r="J15" s="22"/>
       <c r="K15" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L15" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16322,7 +16361,7 @@
       <c r="I16" s="9"/>
       <c r="J16" s="10"/>
       <c r="K16" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="L16" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16355,7 +16394,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="L17" s="12" t="str">
         <f t="shared" si="0"/>
@@ -16470,13 +16509,13 @@
       <c r="I24" s="9"/>
       <c r="J24" s="10"/>
       <c r="K24" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L24" s="12" t="s">
+        <v>505</v>
+      </c>
+      <c r="M24" s="39" t="s">
         <v>506</v>
-      </c>
-      <c r="M24" s="39" t="s">
-        <v>507</v>
       </c>
       <c r="N24" s="7" t="s">
         <v>299</v>
@@ -16824,9 +16863,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5:C6"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16859,85 +16898,115 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>519</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>520</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>522</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>523</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>526</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>523</v>
-      </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>528</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>514</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>534</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>516</v>
-      </c>
-      <c r="C10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>537</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -17002,9 +17071,7 @@
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>399</v>
-      </c>
+      <c r="A23" s="7"/>
       <c r="B23" s="12"/>
       <c r="C23" s="39"/>
       <c r="D23" s="7" t="s">

</xml_diff>